<commit_message>
Updated the Excel file
</commit_message>
<xml_diff>
--- a/abc_model_csv_to_json/abc_csv_input_sample.xlsx
+++ b/abc_model_csv_to_json/abc_csv_input_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monyo\PycharmProjects\ABC_JSON_schema\abc_model_csv_to_json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA448609-11D1-4FD6-B13C-563D96B23F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69405173-1F9D-444F-B9DA-D5331FE981EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" activeTab="1" xr2:uid="{DBF3E41C-67D9-4203-8DB4-BA5359FA276E}"/>
+    <workbookView xWindow="32290" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{DBF3E41C-67D9-4203-8DB4-BA5359FA276E}"/>
   </bookViews>
   <sheets>
     <sheet name="How to get started" sheetId="5" r:id="rId1"/>
@@ -449,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -508,7 +508,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,6 +528,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -559,8 +562,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="647700" y="180975"/>
-          <a:ext cx="9648825" cy="6143625"/>
+          <a:off x="647700" y="184150"/>
+          <a:ext cx="9652000" cy="6248400"/>
           <a:chOff x="3048000" y="219075"/>
           <a:chExt cx="9648825" cy="6143625"/>
         </a:xfrm>
@@ -699,6 +702,79 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1414463</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>152400</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>490538</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>71438</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2049" name="Button 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2049"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="36576" rIns="36576" bIns="36576" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Aptos Narrow"/>
+                </a:rPr>
+                <a:t>Simulate</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -1019,7 +1095,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB648BA0-8A27-4A1B-9AC0-8246946B513D}">
-  <sheetPr>
+  <sheetPr codeName="Sheet4">
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
   <dimension ref="A1"/>
@@ -1036,14 +1112,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFB6778-AC56-47E6-8D0E-51CFA9DE673D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFB6778-AC56-47E6-8D0E-51CFA9DE673D}">
   <sheetPr codeName="Sheet1">
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="B2:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1612,6 +1688,36 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2049" r:id="rId3" name="Button 1">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!Simulate">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>1414463</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>152400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>490538</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>71438</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
@@ -1622,11 +1728,11 @@
   </sheetPr>
   <dimension ref="A1:CO33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="8" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P10" sqref="P10"/>
+      <selection pane="bottomRight" activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2146,10 +2252,10 @@
       <c r="E4" s="11">
         <v>1.3</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" t="s">
         <v>99</v>
       </c>
-      <c r="G4" s="28" t="str">
+      <c r="G4" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -2428,10 +2534,10 @@
       <c r="E5" s="11">
         <v>1.3</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" t="s">
         <v>99</v>
       </c>
-      <c r="G5" s="28" t="str">
+      <c r="G5" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -2710,10 +2816,10 @@
       <c r="E6" s="11">
         <v>1.3</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" t="s">
         <v>99</v>
       </c>
-      <c r="G6" s="28" t="str">
+      <c r="G6" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -2992,10 +3098,10 @@
       <c r="E7" s="11">
         <v>1.3</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" t="s">
         <v>99</v>
       </c>
-      <c r="G7" s="28" t="str">
+      <c r="G7" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -3274,10 +3380,10 @@
       <c r="E8" s="11">
         <v>1.3</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="28" t="str">
+      <c r="G8" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -3556,10 +3662,10 @@
       <c r="E9" s="11">
         <v>1.3</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" t="s">
         <v>99</v>
       </c>
-      <c r="G9" s="28" t="str">
+      <c r="G9" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -3838,10 +3944,10 @@
       <c r="E10" s="11">
         <v>1.3</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" t="s">
         <v>99</v>
       </c>
-      <c r="G10" s="28" t="str">
+      <c r="G10" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -4120,10 +4226,10 @@
       <c r="E11" s="11">
         <v>1.3</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" t="s">
         <v>99</v>
       </c>
-      <c r="G11" s="28" t="str">
+      <c r="G11" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -4402,10 +4508,10 @@
       <c r="E12" s="11">
         <v>1.3</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" t="s">
         <v>99</v>
       </c>
-      <c r="G12" s="28" t="str">
+      <c r="G12" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -4684,10 +4790,10 @@
       <c r="E13" s="11">
         <v>1.3</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" t="s">
         <v>99</v>
       </c>
-      <c r="G13" s="28" t="str">
+      <c r="G13" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -4966,10 +5072,10 @@
       <c r="E14" s="11">
         <v>1.3</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" t="s">
         <v>99</v>
       </c>
-      <c r="G14" s="28" t="str">
+      <c r="G14" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -5248,10 +5354,10 @@
       <c r="E15" s="11">
         <v>1.3</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" t="s">
         <v>99</v>
       </c>
-      <c r="G15" s="28" t="str">
+      <c r="G15" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -5530,10 +5636,10 @@
       <c r="E16" s="11">
         <v>1.3</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" t="s">
         <v>99</v>
       </c>
-      <c r="G16" s="28" t="str">
+      <c r="G16" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -5812,10 +5918,10 @@
       <c r="E17" s="11">
         <v>1.3</v>
       </c>
-      <c r="F17" s="28" t="s">
+      <c r="F17" t="s">
         <v>99</v>
       </c>
-      <c r="G17" s="28" t="str">
+      <c r="G17" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -6094,10 +6200,10 @@
       <c r="E18" s="11">
         <v>1.3</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="F18" t="s">
         <v>99</v>
       </c>
-      <c r="G18" s="28" t="str">
+      <c r="G18" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -6376,10 +6482,10 @@
       <c r="E19" s="11">
         <v>1.3</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="F19" t="s">
         <v>99</v>
       </c>
-      <c r="G19" s="28" t="str">
+      <c r="G19" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -6658,10 +6764,10 @@
       <c r="E20" s="11">
         <v>1.3</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="F20" t="s">
         <v>99</v>
       </c>
-      <c r="G20" s="28" t="str">
+      <c r="G20" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -6940,10 +7046,10 @@
       <c r="E21" s="11">
         <v>1.3</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" t="s">
         <v>99</v>
       </c>
-      <c r="G21" s="28" t="str">
+      <c r="G21" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -7222,10 +7328,10 @@
       <c r="E22" s="11">
         <v>1.3</v>
       </c>
-      <c r="F22" s="28" t="s">
+      <c r="F22" t="s">
         <v>99</v>
       </c>
-      <c r="G22" s="28" t="str">
+      <c r="G22" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -7504,10 +7610,10 @@
       <c r="E23" s="11">
         <v>1.3</v>
       </c>
-      <c r="F23" s="28" t="s">
+      <c r="F23" t="s">
         <v>99</v>
       </c>
-      <c r="G23" s="28" t="str">
+      <c r="G23" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -7786,10 +7892,10 @@
       <c r="E24" s="11">
         <v>1.3</v>
       </c>
-      <c r="F24" s="28" t="s">
+      <c r="F24" t="s">
         <v>99</v>
       </c>
-      <c r="G24" s="28" t="str">
+      <c r="G24" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -8068,10 +8174,10 @@
       <c r="E25" s="11">
         <v>1.3</v>
       </c>
-      <c r="F25" s="28" t="s">
+      <c r="F25" t="s">
         <v>99</v>
       </c>
-      <c r="G25" s="28" t="str">
+      <c r="G25" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -8350,10 +8456,10 @@
       <c r="E26" s="11">
         <v>1.3</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="F26" t="s">
         <v>99</v>
       </c>
-      <c r="G26" s="28" t="str">
+      <c r="G26" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -8632,10 +8738,10 @@
       <c r="E27" s="11">
         <v>1.3</v>
       </c>
-      <c r="F27" s="28" t="s">
+      <c r="F27" t="s">
         <v>99</v>
       </c>
-      <c r="G27" s="28" t="str">
+      <c r="G27" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -8914,10 +9020,10 @@
       <c r="E28" s="11">
         <v>1.3</v>
       </c>
-      <c r="F28" s="28" t="s">
+      <c r="F28" t="s">
         <v>99</v>
       </c>
-      <c r="G28" s="28" t="str">
+      <c r="G28" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -9196,10 +9302,10 @@
       <c r="E29" s="11">
         <v>1.3</v>
       </c>
-      <c r="F29" s="28" t="s">
+      <c r="F29" t="s">
         <v>99</v>
       </c>
-      <c r="G29" s="28" t="str">
+      <c r="G29" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -9478,10 +9584,10 @@
       <c r="E30" s="11">
         <v>1.3</v>
       </c>
-      <c r="F30" s="28" t="s">
+      <c r="F30" t="s">
         <v>99</v>
       </c>
-      <c r="G30" s="28" t="str">
+      <c r="G30" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -9760,10 +9866,10 @@
       <c r="E31" s="11">
         <v>1.3</v>
       </c>
-      <c r="F31" s="28" t="s">
+      <c r="F31" t="s">
         <v>99</v>
       </c>
-      <c r="G31" s="28" t="str">
+      <c r="G31" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -10042,10 +10148,10 @@
       <c r="E32" s="11">
         <v>1.3</v>
       </c>
-      <c r="F32" s="28" t="s">
+      <c r="F32" t="s">
         <v>99</v>
       </c>
-      <c r="G32" s="28" t="str">
+      <c r="G32" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -10324,10 +10430,10 @@
       <c r="E33" s="11">
         <v>1.3</v>
       </c>
-      <c r="F33" s="28" t="s">
+      <c r="F33" t="s">
         <v>99</v>
       </c>
-      <c r="G33" s="28" t="str">
+      <c r="G33" t="str">
         <f>SimInfo!$C$21</f>
         <v>Summer casual</v>
       </c>
@@ -10603,7 +10709,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10614,13 +10720,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B36608F-97F6-4699-877B-F53291F68EEE}">
-  <sheetPr>
+  <sheetPr codeName="Sheet5">
     <tabColor theme="1" tint="0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>